<commit_message>
- Sync designators in BOM with Schematics - Update all production files for the configuration with J-Link
</commit_message>
<xml_diff>
--- a/docs/With J-Link/ZSWatch-Dock.xlsx
+++ b/docs/With J-Link/ZSWatch-Dock.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60988BFB-5A09-40B6-9040-B37187C12E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7849DB65-CF0B-4492-A609-A1D1FB0A6FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="128">
   <si>
     <r>
       <t xml:space="preserve">Nummer
@@ -361,9 +361,6 @@
     <t>ZSWatch-Dock (J-Link included)</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -553,21 +550,12 @@
     <t>R1, R2, R3</t>
   </si>
   <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>R4, R5, R6</t>
-  </si>
-  <si>
     <t>220R</t>
   </si>
   <si>
     <t>R7, R8</t>
   </si>
   <si>
-    <t>5.1k</t>
-  </si>
-  <si>
     <t>Vishay / Dale</t>
   </si>
   <si>
@@ -598,12 +586,6 @@
     <t>855-M20-9990546</t>
   </si>
   <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>GPIO</t>
-  </si>
-  <si>
     <t>X3</t>
   </si>
   <si>
@@ -676,9 +658,6 @@
     <t>Connector_PinHeader_2.54mm:PinHeader_1x05_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>Connector_PinHeader_2.54mm:PinHeader_1x01_P2.54mm_Vertical</t>
-  </si>
-  <si>
     <t>Samtec:SHF-105-01-L-D-SM-TR</t>
   </si>
   <si>
@@ -692,6 +671,9 @@
   </si>
   <si>
     <t>TE Connectivity / P&amp;B</t>
+  </si>
+  <si>
+    <t>5k1</t>
   </si>
 </sst>
 </file>
@@ -815,7 +797,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -852,12 +834,6 @@
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -886,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -961,15 +937,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1296,10 +1263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B31" sqref="B31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1318,10 +1285,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="48.6" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="15"/>
       <c r="D1" s="16"/>
       <c r="E1" s="15"/>
@@ -1331,10 +1298,10 @@
       <c r="I1"/>
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" ht="15">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="22" t="s">
         <v>22</v>
       </c>
@@ -1344,13 +1311,13 @@
       <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" ht="15">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="23">
         <f ca="1">TODAY()</f>
-        <v>45171</v>
+        <v>45196</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -1358,10 +1325,10 @@
       <c r="G3" s="19"/>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="15">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1371,10 +1338,10 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:11" s="10" customFormat="1" ht="15">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="17" t="s">
         <v>14</v>
       </c>
@@ -1432,34 +1399,34 @@
         <v>1</v>
       </c>
       <c r="B8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="20" t="s">
+      <c r="H8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>30</v>
-      </c>
       <c r="I8" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1467,34 +1434,34 @@
         <v>2</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="G9" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>35</v>
-      </c>
       <c r="I9" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1502,34 +1469,34 @@
         <v>3</v>
       </c>
       <c r="B10" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="D10" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="20" t="s">
+      <c r="F10" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="G10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>41</v>
-      </c>
       <c r="I10" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1537,34 +1504,34 @@
         <v>4</v>
       </c>
       <c r="B11" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="D11" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="20" t="s">
+      <c r="G11" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>45</v>
-      </c>
       <c r="I11" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1572,34 +1539,34 @@
         <v>5</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="D12" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="20" t="s">
+      <c r="G12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>50</v>
-      </c>
       <c r="I12" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1607,34 +1574,34 @@
         <v>6</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="20" t="s">
+      <c r="G13" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>54</v>
-      </c>
       <c r="I13" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1642,34 +1609,34 @@
         <v>7</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="D14" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E14" s="20" t="s">
+      <c r="F14" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="G14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>59</v>
-      </c>
       <c r="I14" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1677,34 +1644,34 @@
         <v>8</v>
       </c>
       <c r="B15" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="D15" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="20" t="s">
+      <c r="G15" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>63</v>
-      </c>
       <c r="I15" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1712,34 +1679,34 @@
         <v>9</v>
       </c>
       <c r="B16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="D16" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="E16" s="20" t="s">
+      <c r="F16" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="I16" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1747,34 +1714,34 @@
         <v>10</v>
       </c>
       <c r="B17" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="D17" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="E17" s="20" t="s">
+      <c r="F17" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="G17" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>72</v>
-      </c>
       <c r="I17" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1782,34 +1749,34 @@
         <v>11</v>
       </c>
       <c r="B18" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="D18" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="20" t="s">
+      <c r="F18" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="G18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>77</v>
-      </c>
       <c r="I18" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1817,34 +1784,34 @@
         <v>12</v>
       </c>
       <c r="B19" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="D19" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="20" t="s">
+      <c r="F19" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>81</v>
-      </c>
       <c r="I19" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1852,69 +1819,69 @@
         <v>13</v>
       </c>
       <c r="B20" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="F20" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="20" t="s">
+      <c r="H20" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="G20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="20" t="s">
+      <c r="I20" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="20">
+        <v>14</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="I20" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="K20" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="29">
-        <v>14</v>
-      </c>
-      <c r="B21" s="30" t="s">
+      <c r="C21" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="K21" s="28" t="s">
-        <v>112</v>
+      <c r="D21" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K21" s="20" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1922,34 +1889,34 @@
         <v>15</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="F22" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="G22" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1957,34 +1924,34 @@
         <v>16</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D23" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>93</v>
-      </c>
       <c r="G23" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="I23" s="20" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1992,34 +1959,34 @@
         <v>17</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="F24" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>132</v>
-      </c>
       <c r="G24" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2027,13 +1994,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>99</v>
@@ -2042,129 +2009,84 @@
         <v>100</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" s="20" t="s">
         <v>101</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="28">
+      <c r="A26" s="20">
         <v>19</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" s="28" t="s">
+      <c r="D26" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="I26" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="20">
-        <v>20</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F27" s="20" t="s">
+      <c r="J26" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="K26" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="G27" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="K27" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="20">
-        <v>21</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="I28" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="K28" s="20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="14" customFormat="1" ht="15">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="5"/>
+    </row>
+    <row r="28" spans="1:11" s="14" customFormat="1" ht="15">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" ht="15">
+      <c r="A29" s="24"/>
+      <c r="B29" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+    </row>
+    <row r="30" spans="1:11" s="14" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A30" s="27"/>
+      <c r="B30" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -2174,77 +2096,54 @@
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="15">
-      <c r="A31" s="24"/>
-      <c r="B31" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-    </row>
-    <row r="32" spans="1:11" s="14" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A32" s="27"/>
-      <c r="B32" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" ht="15">
-      <c r="A33" s="25"/>
-      <c r="B33" s="32" t="s">
+      <c r="A31" s="25"/>
+      <c r="B31" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-    </row>
-    <row r="34" spans="1:11" ht="15">
-      <c r="A34" s="26"/>
-      <c r="B34" s="32" t="s">
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+    </row>
+    <row r="32" spans="1:11" ht="15">
+      <c r="A32" s="26"/>
+      <c r="B32" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-    </row>
-    <row r="37" spans="1:11" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="1:11" s="13" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+    </row>
+    <row r="35" spans="1:11" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertRows="0" deleteRows="0" sort="0"/>
   <mergeCells count="9">
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B29:D29"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>

</xml_diff>

<commit_message>
- Fix wrong part number of 10 uH inductor and replace it by the right one
</commit_message>
<xml_diff>
--- a/docs/With J-Link/ZSWatch-Dock.xlsx
+++ b/docs/With J-Link/ZSWatch-Dock.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7849DB65-CF0B-4492-A609-A1D1FB0A6FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD3E819-D0A2-48F7-AEDB-CE86A77EE855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31845" yWindow="3210" windowWidth="13155" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -538,15 +538,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>TAIYO YUDEN</t>
-  </si>
-  <si>
-    <t>LSCNB1608HKT1R0MD</t>
-  </si>
-  <si>
-    <t>963-LSCNB1608HKT1R0MD</t>
-  </si>
-  <si>
     <t>R1, R2, R3</t>
   </si>
   <si>
@@ -674,6 +665,15 @@
   </si>
   <si>
     <t>5k1</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>MLZ1608N100LT000</t>
+  </si>
+  <si>
+    <t>810-MLZ1608N100LT000</t>
   </si>
 </sst>
 </file>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:D31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1317,7 +1317,7 @@
       <c r="B3" s="31"/>
       <c r="C3" s="23">
         <f ca="1">TODAY()</f>
-        <v>45196</v>
+        <v>45238</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -1405,7 +1405,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>27</v>
@@ -1423,10 +1423,10 @@
         <v>23</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1440,7 +1440,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>27</v>
@@ -1458,10 +1458,10 @@
         <v>23</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1475,7 +1475,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>38</v>
@@ -1493,10 +1493,10 @@
         <v>23</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1510,7 +1510,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>38</v>
@@ -1528,10 +1528,10 @@
         <v>23</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1545,7 +1545,7 @@
         <v>47</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>38</v>
@@ -1563,10 +1563,10 @@
         <v>45</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1580,7 +1580,7 @@
         <v>51</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>38</v>
@@ -1598,10 +1598,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1615,7 +1615,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>56</v>
@@ -1633,10 +1633,10 @@
         <v>23</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1650,7 +1650,7 @@
         <v>60</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>56</v>
@@ -1668,10 +1668,10 @@
         <v>23</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1685,7 +1685,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>65</v>
@@ -1703,10 +1703,10 @@
         <v>23</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1720,7 +1720,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>69</v>
@@ -1738,10 +1738,10 @@
         <v>23</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1755,7 +1755,7 @@
         <v>73</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>74</v>
@@ -1773,10 +1773,10 @@
         <v>23</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1790,7 +1790,7 @@
         <v>78</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>79</v>
@@ -1808,10 +1808,10 @@
         <v>23</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1825,28 +1825,28 @@
         <v>25</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1854,34 +1854,34 @@
         <v>14</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>35</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1889,34 +1889,34 @@
         <v>15</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>30</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1924,34 +1924,34 @@
         <v>16</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1959,34 +1959,34 @@
         <v>17</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>96</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1994,34 +1994,34 @@
         <v>18</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2029,34 +2029,34 @@
         <v>19</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="14" customFormat="1" ht="15">

</xml_diff>

<commit_message>
- Fix wrong part number for inductor
</commit_message>
<xml_diff>
--- a/docs/With J-Link/ZSWatch-Dock.xlsx
+++ b/docs/With J-Link/ZSWatch-Dock.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7849DB65-CF0B-4492-A609-A1D1FB0A6FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58DA773-DBA2-46A3-957C-BB723FCF46E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -538,15 +538,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>TAIYO YUDEN</t>
-  </si>
-  <si>
-    <t>LSCNB1608HKT1R0MD</t>
-  </si>
-  <si>
-    <t>963-LSCNB1608HKT1R0MD</t>
-  </si>
-  <si>
     <t>R1, R2, R3</t>
   </si>
   <si>
@@ -674,6 +665,15 @@
   </si>
   <si>
     <t>5k1</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>MLZ1608N100LT000</t>
+  </si>
+  <si>
+    <t>810-MLZ1608N100LT000</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:D31"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1317,7 +1317,7 @@
       <c r="B3" s="31"/>
       <c r="C3" s="23">
         <f ca="1">TODAY()</f>
-        <v>45196</v>
+        <v>45224</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -1405,7 +1405,7 @@
         <v>25</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>27</v>
@@ -1423,10 +1423,10 @@
         <v>23</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1440,7 +1440,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>27</v>
@@ -1458,10 +1458,10 @@
         <v>23</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1475,7 +1475,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>38</v>
@@ -1493,10 +1493,10 @@
         <v>23</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1510,7 +1510,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>38</v>
@@ -1528,10 +1528,10 @@
         <v>23</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1545,7 +1545,7 @@
         <v>47</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>38</v>
@@ -1563,10 +1563,10 @@
         <v>45</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1580,7 +1580,7 @@
         <v>51</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>38</v>
@@ -1598,10 +1598,10 @@
         <v>23</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1615,7 +1615,7 @@
         <v>55</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>56</v>
@@ -1633,10 +1633,10 @@
         <v>23</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1650,7 +1650,7 @@
         <v>60</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>56</v>
@@ -1668,10 +1668,10 @@
         <v>23</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1685,7 +1685,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>65</v>
@@ -1703,10 +1703,10 @@
         <v>23</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1720,7 +1720,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>69</v>
@@ -1738,10 +1738,10 @@
         <v>23</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1755,7 +1755,7 @@
         <v>73</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>74</v>
@@ -1773,10 +1773,10 @@
         <v>23</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1790,7 +1790,7 @@
         <v>78</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>79</v>
@@ -1808,10 +1808,10 @@
         <v>23</v>
       </c>
       <c r="J19" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1825,28 +1825,28 @@
         <v>25</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1854,34 +1854,34 @@
         <v>14</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>35</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1889,34 +1889,34 @@
         <v>15</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>30</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1924,34 +1924,34 @@
         <v>16</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1959,34 +1959,34 @@
         <v>17</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>96</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1994,34 +1994,34 @@
         <v>18</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2029,34 +2029,34 @@
         <v>19</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>26</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>23</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="14" customFormat="1" ht="15">

</xml_diff>